<commit_message>
Change data source to CDC
</commit_message>
<xml_diff>
--- a/data_tndoh/COVID_VACCINE_AGE_GROUPS.XLSX
+++ b/data_tndoh/COVID_VACCINE_AGE_GROUPS.XLSX
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="FINAL_AGEGROUPS"/>
   </sheets>
   <definedNames>
-    <definedName name="FINAL_AGEGROUPS">'FINAL_AGEGROUPS'!$A$1:$H$672</definedName>
+    <definedName name="FINAL_AGEGROUPS">'FINAL_AGEGROUPS'!$A$1:$H$681</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H672"/>
+  <dimension ref="A1:H681"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -16432,7 +16432,7 @@
         <v>266884</v>
       </c>
       <c r="F661" s="0">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="G661" s="0">
         <v>126051</v>
@@ -16516,13 +16516,13 @@
         <v>5100</v>
       </c>
       <c r="F664" s="0">
-        <v>0.562823830623134</v>
+        <v>0.562</v>
       </c>
       <c r="G664" s="0">
         <v>2651</v>
       </c>
       <c r="H664" s="0">
-        <v>0.548795382749069</v>
+        <v>0.548</v>
       </c>
     </row>
     <row outlineLevel="0" r="665">
@@ -16544,13 +16544,13 @@
         <v>61857</v>
       </c>
       <c r="F665" s="0">
-        <v>6.82639091977553</v>
+        <v>6.826</v>
       </c>
       <c r="G665" s="0">
         <v>39569</v>
       </c>
       <c r="H665" s="0">
-        <v>8.19135590343189</v>
+        <v>8.191</v>
       </c>
     </row>
     <row outlineLevel="0" r="666">
@@ -16572,13 +16572,13 @@
         <v>81082</v>
       </c>
       <c r="F666" s="0">
-        <v>8.94801604599705</v>
+        <v>8.948</v>
       </c>
       <c r="G666" s="0">
         <v>52220</v>
       </c>
       <c r="H666" s="0">
-        <v>10.8102960721073</v>
+        <v>10.81</v>
       </c>
     </row>
     <row outlineLevel="0" r="667">
@@ -16600,13 +16600,13 @@
         <v>89785</v>
       </c>
       <c r="F667" s="0">
-        <v>9.90845835931335</v>
+        <v>9.908</v>
       </c>
       <c r="G667" s="0">
         <v>55808</v>
       </c>
       <c r="H667" s="0">
-        <v>11.5530640212977</v>
+        <v>11.55</v>
       </c>
     </row>
     <row outlineLevel="0" r="668">
@@ -16628,13 +16628,13 @@
         <v>100150</v>
       </c>
       <c r="F668" s="0">
-        <v>11.0523150268445</v>
+        <v>11.05</v>
       </c>
       <c r="G668" s="0">
         <v>60462</v>
       </c>
       <c r="H668" s="0">
-        <v>12.5165094046678</v>
+        <v>12.51</v>
       </c>
     </row>
     <row outlineLevel="0" r="669">
@@ -16656,13 +16656,13 @@
         <v>167563</v>
       </c>
       <c r="F669" s="0">
-        <v>18.4918528491577</v>
+        <v>18.49</v>
       </c>
       <c r="G669" s="0">
         <v>52804</v>
       </c>
       <c r="H669" s="0">
-        <v>10.9311925276054</v>
+        <v>10.93</v>
       </c>
     </row>
     <row outlineLevel="0" r="670">
@@ -16684,13 +16684,13 @@
         <v>269568</v>
       </c>
       <c r="F670" s="0">
-        <v>29.7488812496896</v>
+        <v>29.74</v>
       </c>
       <c r="G670" s="0">
         <v>129226</v>
       </c>
       <c r="H670" s="0">
-        <v>26.7516530106116</v>
+        <v>26.75</v>
       </c>
     </row>
     <row outlineLevel="0" r="671">
@@ -16712,13 +16712,13 @@
         <v>130925</v>
       </c>
       <c r="F671" s="0">
-        <v>14.4485705930066</v>
+        <v>14.44</v>
       </c>
       <c r="G671" s="0">
         <v>90304</v>
       </c>
       <c r="H671" s="0">
-        <v>18.6942354748291</v>
+        <v>18.69</v>
       </c>
     </row>
     <row outlineLevel="0" r="672">
@@ -16740,13 +16740,265 @@
         <v>115</v>
       </c>
       <c r="F672" s="0">
-        <v>1.26911255924824E-02</v>
+        <v>0.012</v>
       </c>
       <c r="G672" s="0">
         <v>14</v>
       </c>
       <c r="H672" s="0">
-        <v>2.89820270029686E-03</v>
+        <v>0.002</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="673">
+      <c r="A673" s="0" t="inlineStr">
+        <is>
+          <t>16-20</t>
+        </is>
+      </c>
+      <c r="B673" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C673" s="0">
+        <v>7990</v>
+      </c>
+      <c r="D673" s="0">
+        <v>0.556535742619981</v>
+      </c>
+      <c r="E673" s="0">
+        <v>5261</v>
+      </c>
+      <c r="F673" s="0">
+        <v>0.563728904366461</v>
+      </c>
+      <c r="G673" s="0">
+        <v>2718</v>
+      </c>
+      <c r="H673" s="0">
+        <v>0.545514756796355</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="674">
+      <c r="A674" s="0" t="inlineStr">
+        <is>
+          <t>21-30</t>
+        </is>
+      </c>
+      <c r="B674" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C674" s="0">
+        <v>103730</v>
+      </c>
+      <c r="D674" s="0">
+        <v>7.22521308910771</v>
+      </c>
+      <c r="E674" s="0">
+        <v>63217</v>
+      </c>
+      <c r="F674" s="0">
+        <v>6.77385480846504</v>
+      </c>
+      <c r="G674" s="0">
+        <v>40383</v>
+      </c>
+      <c r="H674" s="0">
+        <v>8.10504872101075</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="675">
+      <c r="A675" s="0" t="inlineStr">
+        <is>
+          <t>31-40</t>
+        </is>
+      </c>
+      <c r="B675" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C675" s="0">
+        <v>136180</v>
+      </c>
+      <c r="D675" s="0">
+        <v>9.48548653691977</v>
+      </c>
+      <c r="E675" s="0">
+        <v>82958</v>
+      </c>
+      <c r="F675" s="0">
+        <v>8.88915081703724</v>
+      </c>
+      <c r="G675" s="0">
+        <v>52965</v>
+      </c>
+      <c r="H675" s="0">
+        <v>10.6303123965118</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="676">
+      <c r="A676" s="0" t="inlineStr">
+        <is>
+          <t>41-50</t>
+        </is>
+      </c>
+      <c r="B676" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C676" s="0">
+        <v>149071</v>
+      </c>
+      <c r="D676" s="0">
+        <v>10.3833967068965</v>
+      </c>
+      <c r="E676" s="0">
+        <v>92093</v>
+      </c>
+      <c r="F676" s="0">
+        <v>9.86798821323332</v>
+      </c>
+      <c r="G676" s="0">
+        <v>56617</v>
+      </c>
+      <c r="H676" s="0">
+        <v>11.3632851308091</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="677">
+      <c r="A677" s="0" t="inlineStr">
+        <is>
+          <t>51-60</t>
+        </is>
+      </c>
+      <c r="B677" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C677" s="0">
+        <v>165141</v>
+      </c>
+      <c r="D677" s="0">
+        <v>11.5027370553199</v>
+      </c>
+      <c r="E677" s="0">
+        <v>103092</v>
+      </c>
+      <c r="F677" s="0">
+        <v>11.0465577283686</v>
+      </c>
+      <c r="G677" s="0">
+        <v>61651</v>
+      </c>
+      <c r="H677" s="0">
+        <v>12.3736314463768</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="678">
+      <c r="A678" s="0" t="inlineStr">
+        <is>
+          <t>61-70</t>
+        </is>
+      </c>
+      <c r="B678" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C678" s="0">
+        <v>234761</v>
+      </c>
+      <c r="D678" s="0">
+        <v>16.3520509978985</v>
+      </c>
+      <c r="E678" s="0">
+        <v>179048</v>
+      </c>
+      <c r="F678" s="0">
+        <v>19.185427270292</v>
+      </c>
+      <c r="G678" s="0">
+        <v>55177</v>
+      </c>
+      <c r="H678" s="0">
+        <v>11.0742706901223</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="679">
+      <c r="A679" s="0" t="inlineStr">
+        <is>
+          <t>71-80</t>
+        </is>
+      </c>
+      <c r="B679" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C679" s="0">
+        <v>412161</v>
+      </c>
+      <c r="D679" s="0">
+        <v>28.7086768728403</v>
+      </c>
+      <c r="E679" s="0">
+        <v>275135</v>
+      </c>
+      <c r="F679" s="0">
+        <v>29.4813822662738</v>
+      </c>
+      <c r="G679" s="0">
+        <v>135587</v>
+      </c>
+      <c r="H679" s="0">
+        <v>27.2129173398629</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="680">
+      <c r="A680" s="0" t="inlineStr">
+        <is>
+          <t>81+</t>
+        </is>
+      </c>
+      <c r="B680" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C680" s="0">
+        <v>226525</v>
+      </c>
+      <c r="D680" s="0">
+        <v>15.7783803625771</v>
+      </c>
+      <c r="E680" s="0">
+        <v>132352</v>
+      </c>
+      <c r="F680" s="0">
+        <v>14.1818376640771</v>
+      </c>
+      <c r="G680" s="0">
+        <v>93133</v>
+      </c>
+      <c r="H680" s="0">
+        <v>18.6922096558922</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="681">
+      <c r="A681" s="0" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="B681" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C681" s="0">
+        <v>108</v>
+      </c>
+      <c r="D681" s="0">
+        <v>7.52263582014492E-03</v>
+      </c>
+      <c r="E681" s="0">
+        <v>94</v>
+      </c>
+      <c r="F681" s="0">
+        <v>1.00723278864184E-02</v>
+      </c>
+      <c r="G681" s="0">
+        <v>14</v>
+      </c>
+      <c r="H681" s="0">
+        <v>2.80986261778844E-03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>